<commit_message>
Absorption BG from Films
</commit_message>
<xml_diff>
--- a/RamanAnalysis/RamanFits/202501_RamanMolecularFilling/FittingResults.xlsx
+++ b/RamanAnalysis/RamanFits/202501_RamanMolecularFilling/FittingResults.xlsx
@@ -29,7 +29,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="36">
+  <borders count="44">
     <border>
       <left/>
       <right/>
@@ -72,11 +72,19 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -113,6 +121,14 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>

</xml_diff>